<commit_message>
result data matrix spreadsheets.
</commit_message>
<xml_diff>
--- a/Additional Resources/Comparison Times Tracker.xlsx
+++ b/Additional Resources/Comparison Times Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andy/Developer/Swansea Uni/CDT/Thesis/CDT_MSc_Thesis/Additional Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3450BBB3-1CDF-5449-BEBF-0F19647CDB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AC8951-AA21-6F45-8DBA-8E0DDAE4F030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18080" windowHeight="28800" xr2:uid="{7227EBF7-96F1-874A-AEE4-6A74659893A3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="18080" windowHeight="28300" xr2:uid="{7227EBF7-96F1-874A-AEE4-6A74659893A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Tweet 1</t>
-  </si>
-  <si>
-    <t>Tweet 2</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,18 +48,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,12 +68,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,137 +384,266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134F07FB-C049-294F-826C-5D85705483FC}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="11" width="5.1640625" customWidth="1"/>
-    <col min="12" max="12" width="5.6640625" customWidth="1"/>
+    <col min="1" max="10" width="5.1640625" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1">
         <v>1</v>
       </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2">
+      <c r="B6">
         <v>8</v>
-      </c>
-      <c r="K2">
-        <v>9</v>
-      </c>
-      <c r="L2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6">
-        <v>4</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>7</v>
       </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>5</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8">
-        <v>6</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -540,139 +652,133 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
         <v>5</v>
       </c>
-      <c r="D9">
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>6</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>6</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>4</v>
-      </c>
-      <c r="I10">
-        <v>4</v>
-      </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11">
-        <v>9</v>
-      </c>
-      <c r="C11">
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
         <v>2</v>
       </c>
-      <c r="D11">
-        <v>6</v>
-      </c>
-      <c r="E11">
-        <v>6</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
-      <c r="H11">
-        <v>7</v>
-      </c>
-      <c r="I11">
-        <v>8</v>
-      </c>
-      <c r="J11">
-        <v>4</v>
-      </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>6</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <v>6</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-      <c r="H12">
-        <v>6</v>
-      </c>
-      <c r="I12">
-        <v>3</v>
-      </c>
-      <c r="J12">
-        <v>4</v>
-      </c>
-      <c r="K12">
-        <v>2</v>
-      </c>
-      <c r="L12" s="2"/>
+      <c r="K11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="A2:A12"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>